<commit_message>
Updated cleaned files and added Raw_Data sheet
</commit_message>
<xml_diff>
--- a/C3/Project_Files/Entertainment Expense.xlsx
+++ b/C3/Project_Files/Entertainment Expense.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="132" yWindow="516" windowWidth="22716" windowHeight="8940" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Entertainment-Expenses---Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Raw_Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Cleaned_Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Entertainment</t>
   </si>
@@ -43,37 +47,45 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,15 +93,15 @@
         <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="4">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -103,38 +115,64 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -142,7 +180,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -332,24 +370,118 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8">
+        <v>95.67</v>
+      </c>
+      <c r="C2" s="8">
+        <v>95.67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8">
+        <v>9.99</v>
+      </c>
+      <c r="C3" s="8">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>32</v>
+      </c>
+      <c r="C4" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8">
+        <v>41.98</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8">
+        <v>132.32</v>
+      </c>
+      <c r="C6" s="8">
+        <v>62.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.38"/>
-    <col customWidth="1" min="2" max="3" width="7.0"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -360,7 +492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -371,7 +503,7 @@
         <v>95.67</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -382,18 +514,18 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -401,34 +533,34 @@
         <v>41.98</v>
       </c>
       <c r="C5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>132.32</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="7">
         <v>62.7</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5">
-        <f t="shared" ref="B7:C7" si="1">SUM(B2:B6)</f>
-        <v>311.96</v>
+        <f t="shared" ref="B7:C7" si="0">SUM(B2:B6)</f>
+        <v>311.95999999999998</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>184.36</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>